<commit_message>
updated JAIS files to reflect final paper results
</commit_message>
<xml_diff>
--- a/examples/HEAT/JAIS_2023/topic_model_results/hazard_extraction_mismatches.xlsx
+++ b/examples/HEAT/JAIS_2023/topic_model_results/hazard_extraction_mismatches.xlsx
@@ -9,8 +9,8 @@
   <sheets>
     <sheet name="Hydraulic Fluid Leaks and Malf" sheetId="1" r:id="rId1"/>
     <sheet name="Intrusion" sheetId="2" r:id="rId2"/>
-    <sheet name="Water Bucket &amp; Tank Equipment " sheetId="3" r:id="rId3"/>
-    <sheet name="Premature Water &amp; Retardant Je" sheetId="4" r:id="rId4"/>
+    <sheet name="Water Drop Bucket or Tank Fail" sheetId="3" r:id="rId3"/>
+    <sheet name="Water or Retardant Loading &amp; J" sheetId="4" r:id="rId4"/>
     <sheet name="Radio Malfunction" sheetId="5" r:id="rId5"/>
     <sheet name="On-board Caution Light Illumin" sheetId="6" r:id="rId6"/>
     <sheet name="Inadequate PPE" sheetId="7" r:id="rId7"/>
@@ -23,7 +23,7 @@
     <sheet name="Personnel Duty Hours Exceeded" sheetId="14" r:id="rId14"/>
     <sheet name="Jumper Operations Hazards" sheetId="15" r:id="rId15"/>
     <sheet name="Control Surface Damage" sheetId="16" r:id="rId16"/>
-    <sheet name="Helitorch Operations Failure" sheetId="17" r:id="rId17"/>
+    <sheet name="Prescribed Burn Operations Fai" sheetId="17" r:id="rId17"/>
     <sheet name="Engine Malfunction" sheetId="18" r:id="rId18"/>
     <sheet name="Oil Malfunction" sheetId="19" r:id="rId19"/>
     <sheet name="Load Limits Exceeded" sheetId="20" r:id="rId20"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="558">
   <si>
     <t>True</t>
   </si>
@@ -748,18 +748,42 @@
     <t>97-0081</t>
   </si>
   <si>
+    <t>01-1095</t>
+  </si>
+  <si>
+    <t>05-0566</t>
+  </si>
+  <si>
     <t>Ordered an infra Red flight of our slash burns for 5/19/97. Was told by the vendor that their radio was not operating and so their helicopter had not been carded as yet. They arranged to use a Bell BIII to complete the flight using a Westcam infra red camera. When I arrived at the vendor's the camera installation was nearly complete and the pilot was waiting for the weights and balance calculations. The Westcam camera is a nose mount weighing 80 lbs. It was determined that you could operate as long as no one was in the left front seat and a 30 gallon fuel reserve was maintained. Mission went foreword with out incident however I have real concerns about the IR mounting system which is a temporary mount: 1) It obviously makes a significant change in aircraft CG and reduces the amount of useable fuel (this mission was flown by a light-weight pilot and I'm not aware of any lighter pilots, a heavier pilot may not have been able to complete this mission). 2) The ground clearance of the camera is approximately 4 inches. This is ok if your operating from a cement pad as this mission was but would be unworkable on most fires or other field operations. 3) No agency personnel were on this flight but on some IR missions it may be desirable. I think this system needs to be looked at before someone decides to do so.</t>
   </si>
   <si>
+    <t>At approximatley 1400 on 09/04/01 Flight Follow when out.  Jumper 59 and Helicopter 70B where both on Initial Attack missions at the time.  Established contact with both aircraft on Air Guard, switched both aircraft to local repeater and completed missions.Contacted local USFS Communications personnel.  He confimed that flight following was broken and would look at it on 09/05/01.Unable to determine when flight follow will be operable due to Communications personnel's response.</t>
+  </si>
+  <si>
+    <t>On my flight from Redmond to Missoula I continuously heard regular business, ground asset dispatching, equipment ordering, and just general chit-chat being done on the National Flight Following Frequency (Come to think of it the frequency could have been the Guard Frequency ).  This use of one or the other frequency is not authorized and did not cease until I was well into Idaho.</t>
+  </si>
+  <si>
     <t>camera</t>
   </si>
   <si>
+    <t>national flight following</t>
+  </si>
+  <si>
     <t>[14, 46, 63, 80, 88]</t>
   </si>
   <si>
+    <t>[14, 29, 69, 74, 97]</t>
+  </si>
+  <si>
+    <t>[3, 69, 80]</t>
+  </si>
+  <si>
     <t>[46]</t>
   </si>
   <si>
+    <t>[69]</t>
+  </si>
+  <si>
     <t>20-1248</t>
   </si>
   <si>
@@ -970,6 +994,9 @@
     <t xml:space="preserve"> tree</t>
   </si>
   <si>
+    <t>snag</t>
+  </si>
+  <si>
     <t>brush</t>
   </si>
   <si>
@@ -1000,510 +1027,492 @@
     <t>[24]</t>
   </si>
   <si>
-    <t>06-0484</t>
+    <t>04-0341</t>
+  </si>
+  <si>
+    <t>07-1118</t>
+  </si>
+  <si>
+    <t>06-0372</t>
+  </si>
+  <si>
+    <t>05-0347</t>
+  </si>
+  <si>
+    <t>02-1091</t>
   </si>
   <si>
     <t>16-0527</t>
   </si>
   <si>
-    <t>95-0286</t>
-  </si>
-  <si>
-    <t>01-0591</t>
-  </si>
-  <si>
     <t>06-0799</t>
   </si>
   <si>
-    <t>01-0112</t>
-  </si>
-  <si>
-    <t>06-0954</t>
-  </si>
-  <si>
-    <t>04-0859</t>
-  </si>
-  <si>
     <t>11-0136</t>
   </si>
   <si>
     <t>06-0673</t>
   </si>
   <si>
+    <t>01-0498</t>
+  </si>
+  <si>
+    <t>20-0256</t>
+  </si>
+  <si>
+    <t>After take-off, acft could not retract left main gear. Flight manual procedures were followed which directed the crew to lower the gear. A safe gear down and locked indication was displayed. Once a safe indication is indicated no further trouble shooting is allowed in flight. Flight engineer visually checked for safe indications thru inspection windows. Retardant was dumped at the fire site due to its proximity. Acft landed at IWA without incident.</t>
+  </si>
+  <si>
+    <t>Flying Fire Managers on Pattengail Fire Recon. Air Attack~above helicopters~air attack complained they could not see me on TCAS, but could see the helicopters below me. Reason is the helicopter''s transponder attenna is housed in plexiglass nose which transmits through. My transponder attenna is on the bottom of my fuselage. Air attack above me could not see me on TCAS as signal won''t go through aluminum fuselage.</t>
+  </si>
+  <si>
+    <t>Upon touchdown at Helibase, the aircraft bounced on wheels and skidded approx. 15 feet before coming to a stop. Crew was unloaded along with gear at Helibase. PIC did a walkaround of aircraft looking at wheels, landing struts, etc. inspecting for any damage, none found. Aircraft was later inspected by mechanics at airport and no damage was found. Upon review of load calculation it was found that aircraft was overloaded approx. 450 pounds for conditions at site. The Helibase was an inground location. Pilot directed aircraft into the wind for landing as per normal. Performance planning was not accurate for actual conditions at Helibase. This responsibility lies with the Helicopter manager who accepts responsibility for incident. We did not confirm actual conditions before landing as is normal SOP, I believe we were mission focused as the fire was in close proximity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We departed KSBA at 0830 on an infra-red flight over the Xxxxxxx incident. The weather at departure was IFR, light wind out of the west, 5 miles visibility and a ceiling of 500’ with tops reported at 1500’with VFR conditions on top. The mission took roughly 45 minutes over the incident, and we returned to KSBA under VFR conditions. Weather at the time of landing was reported at 6 miles visibility with ceilings of 600’ tops remained at 1500’. After receiving an IFR clearance, we were cleared for the ILS 7 approach to KSBA. I armed the approach mode of the flight director while hand flying the aircraft. The flight director did not seem to capture the localizer, and I intercepted the course with the HSI. Glide slope information appeared normal. I informed SBA approach that I may not have a good signal. At this time I was handed to tower and cleared to land. The tower informed me that I was slightly right of course; this appeared to agree with the GPS moving map. However, this information conflicted with both the flight director and the HSI which were showing opposing information and large fluctuations in course corrections. At this time the TWAS issued a “terrain pull up” alert at 1100’AGL. I initiated a missed approach and climbed back up to VFR conditions diverting to KPRB. Some fluctuations in the HSI were observed while in route, and the landing was without incident. R-5 Aviation Maintenance Inspector was called 7/3/2005. R-5 Contracting Officer was called 7/3/2005. The plane was later ferried to KFAT under VFR conditions for maintenance. </t>
+  </si>
+  <si>
+    <t>Helicopter NXXXXX (H-52) was assigned to the Big Wash fire on 6-6-02 (Cedar City BLM). H-52 was reconing division W with Operations and the Safety Officer. Air attack 69 November was on station along with helicopter Hotel Tango and Hotel Quebec (who where doing bucket work for division W). H-52 was orbiting Division W at 9000' MSL and coordinating with division (on air to ground). The elevation of the fire being around 8400'. While watching helicopter Hotel Tango returning from a drop, an unidentified fixed wing underflew H-52 going southbound (Later identified as Lead 44). Neither H-52 or helicopter Hotel Tango had heard that Lead 44 was in the area. When H-52 inquired to air attack about other fixed wing in the area, Air Attack responded in Lead 44in.</t>
+  </si>
+  <si>
+    <t>On July 8 2016 19:10 a Temporary Flight Restriction {TFR} intrusion occurred on the XXX Fire near Pine Valley Utah involving an Unmanned Aircraft System {UAS} or drone. This TFR intrusion resulted in a near collision with Air Attack XXX. XXX was at an altitude of 11,000 feet when they passed the drone 30 feet off the right wing of the plane. The incident occurred on the XXX Fire at approximately LAT/LONG 37 23 .104 113 31.149. Geographical location of Lloyds canyon and Forsythe Canyon on the Pine Valley Mountain range. This is the forth confirmed UAS intrusion on this fire.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At 1751, MDC called and told me T-xx was en route from WYS to the incident, but that the fire had cancelled them. They wanted HLN aircraft to call T-xx and have him go directly to MSO instead of to the incident. AFF showed T-xx just SW of HLN. I called him on National Flight Following - no response at 1752. Tried again, 1753 - no response. 1753 - AIR GUARD contact attempted. No response. 1754, Tried contact on National Flight Following and again on AIR GUARD - no response. Icon went red on Automated Flight Following (AFF) screen. 1757, tried AIR GUARD again. No response. Called the HLN Tower. They had not seen T-xx in the skies (HLN tower does not have radar). A leadplane tried to raise him on NFF and on 125.125 (receiving incident''s Air-Air). I told Leadplane that the last point I had him on AFF was at 1739 (note time there - it is now 1758 on the clock), and relayed the last known position check: lat/long, heading 337 degrees @ 247 mph. Had MDC on the phone (to check the status of T-xx as far as they knew). They reported T-xx was ''yellow'' on their screen - relayed to leadplane. Moments later, MDC reported he''d gone ''red'' on her screen too. Relayed to Leadplane. Moments later, the lead successfully established contact with the tanker, who reported he was almost to the fire. HDC dispatcher checked with our Forest Aviation Officer, the GACC a/c desk (NRCC), neighboring dispatch center involved (MDC), as well as my center manager (HDC). All suggested a Safecom be filed for a number of related reasons, all centering on the fact that Air Guard is to be monitored at all times in aircraft, even when said a/c are employing Automated Flight Following. </t>
+  </si>
+  <si>
+    <t>While enroute to the Duke Fire and West of Midland Texas the pilot tried to adjust the pitch on the {{{{{#}}}}}2 engine prop. The prop control failed at 2200 rpm. The pilot made the decision to return to Midland International Airfield to have the prop control checked. He then contacted the company mechanic who was enroute to meet the A/C in Midland. The mechanic found a broken wire at a solder point.</t>
+  </si>
+  <si>
+    <t>On July 20th at approximately 0916 air attack departed Redmond Tanker base to respond to Incident #0521 with pilot, air attack trainee and air attack instructor on board. Immediately after take-off, pilot in command informed air attack that we have a mechanical problem and we are returning to Redmond. After landing pilot informed air attack that the fuel flow gauge was inoperable and that he will take the plane to the local A&amp;P mechanic to inspect faulty gauge.</t>
+  </si>
+  <si>
+    <t>Aircraft was observed flying from the Northwest, divert directly over the fireon one wing and depart the area to the southeast. Altitude was approximately 1000' AGL or 6000' MSL. Air tankers were working on the fire. The Roosevelt A &amp; B MOA curently extends from 11,000' MSL to Fl 180.Aircraft obviously deviated from original flight route to investigate the fire (against AP-1B instructions).Aircraft was obviously well below the floor of the MOA.</t>
+  </si>
+  <si>
+    <t>We, the smokejumper aircraft took runway 24 for takeoff and made our departure call on UNICOM.  Helitack helicopter said on UNICOM they were lifting from the ramp and would hold for our takeoff.  We started our takeoff roll and the helicopter departed to the north crossing runway 24 approximately 4,000 feet in front of us.  We called on UNICOM that we were already on our takeoff roll and the helicopter stated that they had us in sight.</t>
+  </si>
+  <si>
+    <t>proximity</t>
+  </si>
+  <si>
+    <t>conflict</t>
+  </si>
+  <si>
+    <t>collision</t>
+  </si>
+  <si>
+    <t>confusion</t>
+  </si>
+  <si>
+    <t>airfield</t>
+  </si>
+  <si>
+    <t>trainee</t>
+  </si>
+  <si>
+    <t>[21, 30, 69, 83]</t>
+  </si>
+  <si>
+    <t>[40, 73, 80, 88]</t>
+  </si>
+  <si>
+    <t>[3, 63, 80, 88]</t>
+  </si>
+  <si>
+    <t>[13, 46, 69, 96]</t>
+  </si>
+  <si>
+    <t>[7, 12, 69, 78, 91]</t>
+  </si>
+  <si>
+    <t>[7, 37]</t>
+  </si>
+  <si>
+    <t>[38, 65]</t>
+  </si>
+  <si>
+    <t>[8, 22, 51, 92]</t>
+  </si>
+  <si>
+    <t>[8, 11]</t>
+  </si>
+  <si>
+    <t>[7, 14, 23, 57, 97]</t>
+  </si>
+  <si>
+    <t>[7, 8, 82]</t>
+  </si>
+  <si>
+    <t>[69, 96]</t>
+  </si>
+  <si>
+    <t>[47, 39]</t>
+  </si>
+  <si>
+    <t>[12, 69, 7]</t>
+  </si>
+  <si>
+    <t>[37, 7]</t>
+  </si>
+  <si>
+    <t>[65]</t>
+  </si>
+  <si>
+    <t>97-0124</t>
+  </si>
+  <si>
+    <t>I was air attack Group Supervisor (AA6) flying over fire B441 talking to jump 17. We assigned them an altitude to come over the fire for a streamer pass while the air tanker was reloading. Jump17 finished his streamer run and started to climb without talking to us. We had jump 17 in sight at all times. Jay requested the pilot to notify air attack prior to changing elevations.</t>
+  </si>
+  <si>
+    <t>streamer</t>
+  </si>
+  <si>
+    <t>[34]</t>
+  </si>
+  <si>
+    <t>20-0733</t>
+  </si>
+  <si>
+    <t>01-0465</t>
+  </si>
+  <si>
+    <t>Approaching SBD for a load and return to the XXXXX Fire, TXXX had a bird strike on the underside of the right wing with damage to the outer flap tab hinge fairing. There was no damage to the actual mechanism.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While flying recon on the Plumas NF I was about to call dispatch with adirection change when I noticed that radio #3 had gone off. I then triedto talk to the pilot and was unable to. I got his attention and then wenoticed that radio #2 had gone off. We then noticed the victor radio wasoff. We then started checking and found that the amp guage was showing adischarge. I called dispatch on my hand held radio and informed them thatwe lost the aircraft alternator and were in route to Quincy (Gansner)airport. The pilot turned off all other unnecessary electrical equipmentto save as much battery life as possibe. We were able to make a safe landing at Quincy airport even though we did not have any flaps. </t>
+  </si>
+  <si>
+    <t>flap</t>
+  </si>
+  <si>
+    <t>[2, 21, 23, 25]</t>
+  </si>
+  <si>
+    <t>[11, 14, 46, 74, 90]</t>
+  </si>
+  <si>
+    <t>[23]</t>
+  </si>
+  <si>
+    <t>18-0517</t>
+  </si>
+  <si>
+    <t>05-0559</t>
+  </si>
+  <si>
+    <t>06-0519</t>
+  </si>
+  <si>
+    <t>15-0631</t>
+  </si>
+  <si>
+    <t>09-0269</t>
+  </si>
+  <si>
+    <t>01-0299</t>
+  </si>
+  <si>
+    <t>02-0566</t>
+  </si>
+  <si>
+    <t>16-0289</t>
+  </si>
+  <si>
+    <t>03-0497</t>
+  </si>
+  <si>
+    <t>16-0706</t>
+  </si>
+  <si>
+    <t>06-0331</t>
+  </si>
+  <si>
+    <t>08-0326</t>
+  </si>
+  <si>
+    <t>03-0781</t>
+  </si>
+  <si>
+    <t>00-0163</t>
+  </si>
+  <si>
+    <t>07-0833</t>
+  </si>
+  <si>
+    <t>11-0806</t>
+  </si>
+  <si>
+    <t>08-0578</t>
+  </si>
+  <si>
+    <t>11-0174</t>
+  </si>
+  <si>
+    <t>04-0434</t>
+  </si>
+  <si>
+    <t>02-0758</t>
+  </si>
+  <si>
+    <t>07-0608</t>
+  </si>
+  <si>
+    <t>16-0815</t>
+  </si>
+  <si>
+    <t>00-0698</t>
+  </si>
+  <si>
+    <t>13-0416</t>
+  </si>
+  <si>
+    <t>03-0192</t>
+  </si>
+  <si>
+    <t>03-1106</t>
+  </si>
+  <si>
+    <t>19-0126</t>
+  </si>
+  <si>
+    <t>WADNR UH-1H xxxxx was dispatched to the Ryegrass Coulee fire in the vicinity of Vantage, WA at 0730, 07/10/2018. xxxxx flew one fuel cycle and then landed at the helibase/ fuel site for a fuel and hold. At approximately 11:00 Air Attack requested xxxxx for bucket work, while lifting to leave the helibase a chip detector and warning light activated. The pilot contacted air attack and informed him the aircraft would be down for maintenance. xxxxx set down at the helibase, contacted agency mechanics and went through the proper procedures to isolate and remedy the issue. After the appropriate steps were taken the agency mechanic cleared xxxxx for incident operations. The aircraft finished up the day and returned to ellensburg base with no further issues.</t>
+  </si>
+  <si>
+    <t>NXXXX was flying air attack on the Burnt River Complex, over incident 154, call dispatch with a report that they lost an engine and were going to try to fly back to Baker on a single engine. At the time of engine failure, they were 22 miles out of Baker. Maintained Contact with NXXXX throughout the flight to Baker. They were able maintain altitude and land safely @ Baker without incident.Contacted Forest Aviation Officer and vendor. Also requested emergency response at the Baker Airport.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pilot failed to untie main rotor blades before start up. Pilot noticed that he did not untie at the same time he attempted to start engine. Immediately aborted start. Total time was approximately one second. Pilot untied blades and started helicopter. </t>
+  </si>
+  <si>
+    <t>Turbocharged 337 Cessna Skymaster pilot started the front engine without any problems. Attempted to start the rear engine but it would not start. The pilot followed other starting procedures as recommended by the owner but without success. The company mechanic was contacted and it was determined the fuel pump had failed. At 1900 aircraft was unavailable.</t>
+  </si>
+  <si>
+    <t>The helicopter departed CKX and upon arrival at the fire several warning lights{particle separator, rpm, engine 1 out, and engine 2 out} became illuminated. The pilot immediately began maneuvering toward the nearest landing spot, but all other gauges read normally &amp; we could still hear the engines running, so we returned to CKX. Enroute all warning lights except one paticle separator light went out. The helicopter landed without incident and the mechanic, IC, and AMD maintenance inspector were notified of the problem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanker 14 was responding to the Silent fire (RRU-47545) and developed an oil leak at the number three engine.  Tanker 14 then returned to SBD Tanker Base.  After inspection it was noted that an oil line was loose.  Oil line tightened, and aircraft put into contract availability.Gerry Burney notified and approved. </t>
+  </si>
+  <si>
+    <t>Dispatched as initial attack to a fire. Started acft engine and all appeared normal until the gas produced tachometer (N) went through 40%,I released the started switch and the engine flamed out, all indicationsof the start up to that point were normal.I contacted the DNR mechanic supervisor and he thought that perhaps thethrottle was rolled back a little to far off the detent to continuestarting sequence. Also, he said that there was the possibility of something similar to a vapor lock (air bubble) may have occured.I attempted a restart at his request and everything performednormally.After the restart Helicopter Manager contacted DNR Mechanic Supervisor once again to obtain clearance to resume operations. Clearancewas granted by mechanic.Helibase Manager contacted USFS to discuss start difficulties. After a conference between FS and DNR representatives Rotor 338 was fullyoperational.</t>
+  </si>
+  <si>
+    <t>We left the Airtanker Base at 1046 to do a requested Recon mission over the Galeuros and the Chirichua Ranges. We finished the Galeuros and were at the Dos Cabezas Mountains enroute to the Chrichuas when the pilot alerted me that the right engine tachometer needle was falling. I looked at the gauges and was a slow descent to 0 rpms. The pilot checked all the other gauges and they were all in the green. I visually looked at the right engine which showed no outward abnormalities. The pilot said that the xxx airport was close and we agreed that we would head the aircraft to there. Once that decision was made I called Dispatch and informed them that we had a malfunction with one of the gauges but operations were good and we were proceeding to the airport. We landed and went to maintenance facilities. Once parked, I notified Dispatch we were safe on the ground, and then notified management, and the OAS Maintenance Inspector of the situation.</t>
+  </si>
+  <si>
+    <t>Assign to lighting recon flight at 1050 Hrs. At end of planned flight, pilot noted right engine HP would not come back below 250 HP. Made landing at SBA at 1200 hrs. Mechanic worked on aircraft with test flight being OK. SZ Aviation Maintenace Inspector was called and aircraft was return to availability status. At 1549 hrs response to SB co fire #5209. 1615 hrs right engine would not come back below 250 HP, landed at SBA at 1641 hrs. SZ Maintenance Inspector was called on the situation, log book entry will be fax to Jerry when aircraft is returned to availability status.</t>
+  </si>
+  <si>
+    <t>Bird strike on engine number 1 noticed by crew chief on walk-around and discontinued reload for fire. Operations shut down. Pilots did not notice any engine concerns. Do not know the altitude, coordinates of strike or time it happened.</t>
+  </si>
+  <si>
+    <t>Aborted start on fire dispatch. Pilot attempted to start the aircraft with the battery cart. Initial voltage OK, upon spooling engine pilot noted excessive voltage drop. Not enough battery voltage to continue start. Pilot verified condition - low NG speed. Pilot followed proper procedure and correctly aborted start without any damage to aircraft.</t>
+  </si>
+  <si>
+    <t>On 6.16.2008 at approximately 1730 airtanker Lockheed P2 Neptune tail number xx was in the blocks and was under supervision of fixed wing parking tender. Aircraft had just completed loading retardent, loading crew was cleared, and airtanker was given permission to start engines. Pilot signaled to FWPT to clear him to start engine {#}2, clearance was given. As engine {#}2 was starting the suction from the propeller sucked a collapsible fabric and wire sunscreen out of the copilots window. The sunscreen disappeared with the engine blowby smoke behind the aircraft. Clearance was asked and given to start engine {#}1. As engine {#}1 cleared of smoke the sunscreen reappeared and swirled with the engine turbulence, threatening to be sucked into engine air intakes of both engine {#}1 and engine {#}2. Parking tender gave the pilot an emergency immediate cut-engine signal. Pilot responded immediately. The sunscreen fell to the ground in front of engine {#}2 and was retrieved by FWPT.</t>
+  </si>
+  <si>
+    <t>Pilot reported low fuel pressure indicator illuminated on the number 4 engine while over fire preparing for a drop.  PIC elected not to drop and returned to MFR for repairs.   Aircraft landed without incident.</t>
+  </si>
+  <si>
+    <t>After landing at KGCN for fuel the cowl of the right engine was observed to have a coating of grease that appeared to have come from the area of the propeller hub.  The aircraft had returned from spending 3.5 hours conducting leadplane activities on the Outlet Fire.</t>
+  </si>
+  <si>
+    <t>On takeoff fuel pressure gauges read normal, 10 minutes into the flight the right engine fuel pressure gauge was reading high. So the pilot decided to terminate the flight on return to the airport. aircraft was placed into contract unavailable status. Company maintenance chief decided to replace the right engine driven fuel pump and do the scheduled 50 hr inspection at the same time. During the inspection the mechanic found the right engine driven hydraulic pump had failed. Hydraulic pump was replaced 8/8/07.</t>
+  </si>
+  <si>
+    <t>Aircraft had an ‘Engine’ chip light starting up at Spring Creek Helibase and immediately shut back down.</t>
+  </si>
+  <si>
+    <t>Pilots heard a noise in the aft rotor system and a vibration upon returning to helibase, the aircraft was shut down while it was inspected by the mechanics, after inspection the mechanics advised the manager that the aircraft was out of service. There was a scheduled maintance to change the aft transmission the next day. The aircraft was made unavailable for the remainder of the afternoon.</t>
+  </si>
+  <si>
+    <t>After flying 4.6 hours on the Rockhouse Fire a transmission oil pressure warning light illuminated but transmission pressure indications were normal. Warning light is turned on by two pressure switches, one plumbed to the forward transmission and one on the aft transmission. This occured upon startup after refueling.</t>
+  </si>
+  <si>
+    <t>While performing large fire support on the Incident, an oil leak was discovered. Oil was dripping out of the valve and pooling in the carriage. 7/2/04 This narrative is an ammendment to the SAFECOM filed for this helicopter on 6/30/2004 (submitted by Helicopter Manager). Narrative: While performing a longline hookup I noticed a couple of puffs of white smoke come out of the left side cowl. I immediately had the pilot land and shut down the A/C. Upon inspection a leak was discovered on the breather tube flange that returns excess oil to the exhaust to be burned off. After discussion with the pilot it was determined that the helicopter needed to be repaired and that it would become un-available. I discussed the problem with my HELB(t) and we decided one of us needed to return to helibase to begin working on getting the helicopter repaired. The HELB(t) flew to helibase with the A/C. While I had confidence in the judgement of the pilot that the leak did not jeopardize the safety of the flight, I should have not asked the HELB(t) to fly down with the ship. This was a MAJOR oversight on my part. Policy dictates that when a problem is discovered that the A/C becomes unavailable @ that point. Once unavailable NO government personnel should be transported until the A/C is returned to service by an appropriate maintenance inspector.</t>
+  </si>
+  <si>
+    <t>Pilot reported low torque, inspection revealed fuel stream from P1 port in the inlet.  P1 bellows cracked.  Removed fuel control, installed fuel control with Allied Signal 1330.2 manual, chapter 73.  Put back into contract availability by the Regional Aviation Maintenance Inspector.</t>
+  </si>
+  <si>
+    <t>Pilot stated that he had an Engine/Airframe/Oil Filter Chip Light while on a Initial Attack mission. Pilot landed the aircraft and checked the chip plug and found very light fuzz on the plug. Pilot is an A/P mechanic.</t>
+  </si>
+  <si>
+    <t>Pilot attempted start of aircraft with main rotor tie down still in place. It was recognized prior to light off of engine by crew followed by immediate shut-down of starter generator.</t>
+  </si>
+  <si>
+    <t>The helicopter was getting ready to start and depart for the project site.  The pilot tried to start the helicopter and it did not.  He tried a second time and was uncessful.  He motioned to the fuel truck driver to bring out the APU and hook it up.  The pilot then tried a thrid time and determined the ignitor had gone bad.  Pilot called the office and had a mechanic dispatched.  A maintenance inspector was contacted and he said that in order to put the helicopter back in service the ignitor would have to be replaced and make a entry in the log book.</t>
+  </si>
+  <si>
+    <t>On duty at 0900, this would be day 3 for mission over site for the Fire within the Zone. At 0920 we did a aircraft systems check before departure and all ops normal, at 0941 we departed airport for the incident with: two souls, 4 1/2 hours of fuel, on a heading 214 degree`s for a 22 min, ETE to the incident. at this point all operations were normal and during this time was calculating the times for relief air attack over the fire. At 12 miles from incident contacted IA helicopter on victor for entry into the airspace of the fire TFR in place, we proceeded into the area at 10,000 dropping to 9,000 ft all ops normal. Established ground contact with operations and IC for operational update and reconfiguration of divisions from the previous day. ordered up fixed wing aircraft: 2 seats for retardant line across the west flank of the fire towards the head. All ops normal. about 3 3/4 hours into the flight the pilot noticed that the fuel use gauge that reads pounds of fuel used per sec was not operational for the right engine, the engine never quit running. The pilot re-calculated the weights and measures for passenger, fuel and cargo, determined that it was either a gauge failure or sending unit and we had plenty of fuel. At 1348 air attack relief was over the fire, did a brief on the tactics and division break downs and handed off to the relief air attack. We proceeded back to The designated base, all ops normal except for the faulty reading of the right fuel/use gauge. Landed safely, notified UAM and Dispatch that aircraft was unavailable due to gauge failure.</t>
+  </si>
+  <si>
+    <t>On the 2nd load of the morning, with the 2nd stick of rappellers, the engine fuel pump caution light came on.  The indicator light came on while the rappellers were on the skids, ready to exit the aircraft.  The pilot notified the spotter after the rappellers were on the ground and off the ropes, due to the fact that there was no fluctuation in fuel pressure.  The spotter disconnected ropes, closed doors and returned to the helipad.  Helicopter was then shutdown for inspection.</t>
+  </si>
+  <si>
+    <t>After refueling in Ely Nevada, XXX was enroute back to Battle Mountain Nevada.  Two minutes outside of Battle Mountain the pilot and I noticed the aroma of fuel.  Upon landing in Battle Mountain, we were in the process of parking the aircraft and noticed a fuel leak on the right side engine.  The pilot shut down the aircraft and made his inspections.  The problem appeared to be a broken fuel line.  The pilot then made calls to his company and mechanics.  I notified Battle Mountain Dispatch, WGBCC and Boise Smokejumpers Duty Officer.  Returned to service 7/1/03.  All repairs done at 0800.</t>
+  </si>
+  <si>
+    <t>As we were coming in to the LZ, one of the crew members on the ground noticed something leaking by the fuel tank. Once we landed and shut the helicopter down the pilot came and examined the leak. He said it was for sure fuel and we needed to find out where it was coming from. The pilot looked into the engine a little more and found out it was leaking between the electric fuel shut off valve. The pilot pressurized the system with the boost pumps and could not recreate the leak. He returned to base without the helitack crew.</t>
+  </si>
+  <si>
+    <t>engine</t>
+  </si>
+  <si>
+    <t>transmission</t>
+  </si>
+  <si>
+    <t>white smoke come</t>
+  </si>
+  <si>
+    <t>generator</t>
+  </si>
+  <si>
+    <t>[33, 41, 50]</t>
+  </si>
+  <si>
+    <t>[7, 11, 59, 65, 69]</t>
+  </si>
+  <si>
+    <t>[29, 83]</t>
+  </si>
+  <si>
+    <t>[7, 88]</t>
+  </si>
+  <si>
+    <t>[73, 82, 85]</t>
+  </si>
+  <si>
+    <t>[8, 14, 67, 71, 97]</t>
+  </si>
+  <si>
+    <t>[55, 80, 83, 97]</t>
+  </si>
+  <si>
+    <t>[21, 43, 82]</t>
+  </si>
+  <si>
+    <t>[25, 41]</t>
+  </si>
+  <si>
+    <t>[13, 83]</t>
+  </si>
+  <si>
+    <t>[2, 8, 50, 88]</t>
+  </si>
+  <si>
+    <t>[8, 11, 41]</t>
+  </si>
+  <si>
+    <t>[3, 14, 23, 69, 97]</t>
+  </si>
+  <si>
+    <t>[53, 67, 82]</t>
+  </si>
+  <si>
+    <t>[80, 93]</t>
+  </si>
+  <si>
+    <t>[24, 74]</t>
+  </si>
+  <si>
+    <t>[50, 53, 58, 85]</t>
+  </si>
+  <si>
+    <t>[64, 67, 68, 80]</t>
+  </si>
+  <si>
+    <t>[7, 23, 43, 97]</t>
+  </si>
+  <si>
+    <t>[50, 80]</t>
+  </si>
+  <si>
+    <t>[11, 22, 58, 68, 97]</t>
+  </si>
+  <si>
+    <t>[63, 83]</t>
+  </si>
+  <si>
+    <t>[3, 41, 53, 97]</t>
+  </si>
+  <si>
+    <t>[8, 53, 67]</t>
+  </si>
+  <si>
+    <t>[41, 67, 88]</t>
+  </si>
+  <si>
+    <t>[50, 41]</t>
+  </si>
+  <si>
+    <t>[8, 97]</t>
+  </si>
+  <si>
+    <t>[83, 97]</t>
+  </si>
+  <si>
+    <t>[41]</t>
+  </si>
+  <si>
+    <t>[50, 8]</t>
+  </si>
+  <si>
+    <t>[8, 41]</t>
+  </si>
+  <si>
+    <t>[97]</t>
+  </si>
+  <si>
+    <t>[50]</t>
+  </si>
+  <si>
+    <t>[64]</t>
+  </si>
+  <si>
+    <t>[41, 97]</t>
+  </si>
+  <si>
+    <t>00-0509</t>
+  </si>
+  <si>
+    <t>Subject:  SAFECOM - Canadian Bird Dog#52,           Left Engine Failure.At approximately 1100 hours MDT Canadian Bird Dog#52, a Turbo Commander, departed Miles City, Montana for Helena, MT.  After reaching cruising altitude of 12,500 feet westbound, and 25 minutes out of Miles City, the left engine suddenly lost power and went to auto feather.  There were no prior indications (instrumentation) that there was a problem developing.  After a cool down period of approximately 2 minutes, and attempt to restart the engine was made but immediately aborted due to no indication of oil pressure.The aircraft was under FS flight following with Lewistown as Billings could not be raised.  Flight following and position reports were also conveyed to Helena on FS nets.The aircraft had no difficulty maintaining altitude and was operating in CAVU conditions.  The flight crew made a judgement call to continue on to Missoula where they had maintenance support even though it was somewhat further than Helena where the logistics of repair would be difficult.  This decision was based on what the flight crew believed to be inpracticablein given the circumstances of clear air, no problems in maintaining altitude, other available landing places along the route, and the availability of maintenance support in Missoula.Bird Dog #52 continued west at 12,500 feet MSL with no further difficulties, other than reduced airspeed, and maintained visuals on airports and landing area's they could reach if problems developed with the right engine.Landing was affected in Missoula at near 1200 hours where they taxied to Northstar Aviation and met with their maintenance team.  The cowling was removed, screens pulled showing a lot of evidence of metal particle, i.e., steel and brass.  The engine had failed and required an engine change.USDA Forest Service LiaisonCanadian Airtanker Deployment</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>[8, 14, 62, 80, 82]</t>
+  </si>
+  <si>
+    <t>07-0629</t>
+  </si>
+  <si>
     <t>03-0668</t>
   </si>
   <si>
-    <t>20-0256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At 1646 local time, two Panavia Tornado fighter jets passed through the Bear Fire TFR at low level (&lt;500 feet AGL) at a high rate of speed (&gt;250 knots estimated) travelling west to east. The two jets were painted in a dark gray paint scheme much darker than the USAF gray paint. Air attack was just entering the area. Ground personnel including the AOBD and team ATGS witnessed the intrusion from Bear ICP which was overflown by the trailing jet in the pair. The Bear Fire was covered at the time by NOTAM Number : FDC 6/0867 . </t>
-  </si>
-  <si>
-    <t>On July 8 2016 19:10 a Temporary Flight Restriction {TFR} intrusion occurred on the XXX Fire near Pine Valley Utah involving an Unmanned Aircraft System {UAS} or drone. This TFR intrusion resulted in a near collision with Air Attack XXX. XXX was at an altitude of 11,000 feet when they passed the drone 30 feet off the right wing of the plane. The incident occurred on the XXX Fire at approximately LAT/LONG 37 23 .104 113 31.149. Geographical location of Lloyds canyon and Forsythe Canyon on the Pine Valley Mountain range. This is the forth confirmed UAS intrusion on this fire.</t>
-  </si>
-  <si>
-    <t>At approximately 1444 on 7/31/95 the incident commander on the Pilot Fire (X-051) called Elko Interagency Dispatch Center and reported to the aircraft desk that five jets flew directly over their fire at an elevation of 1000 feet AGL and below.  We had a TFR issued to us for this area notam #5/3745.  This was a sensitive area as it was in a MOA and on the edge of a restricted area so we made ample notification both by phone and fax to both the FAA and the military unit responsible for the scheduling of the air space.  I called the Hill Command Post and spoke with the supervisor who said that they had some Air Force Reserve jets flying in the area they were briefed on the TFR in effect for the fire.  He said he would make an investigation and submit a report to the BLM State Aviation Manager.  It was fortunate that the two helicopters doing crew shuttles and bucket work on this fire were both on the ground getting ready to take off at the time of the intrusion.  The jets were flying below some of the crews working the ridges around the fire.  This type of incident has serious potential and is an on going problem with the military.</t>
-  </si>
-  <si>
-    <t>A TFR 91.137 violation was reported by helibase manager and helicopter NXXX.  A yellow SuperCub landed at Spanish Fork Airport (U77) and was ingreetedin by the ASGS for Type 1 Team.  I asked the pilot if he was flying over Payson Canyon and Walker Flats.  He admitted he was, but when he saw the helicopter he left the vicinity.  He further stated that he thought the fire was out.  I asked him if he circled over Payson Helibase and he said no, it was a white Husky.  I then asked the NYYYY pilot if he had checked the NOTAMS for TFR's.  He said no, he had not checked any NOTAMS.  I then stated that it was required the myself, as the ASGS, to file a SAFECOM for the incident.  The pilot said inFine, notify the FAAin, inBring 'em on!in.  I further stated that TFRs are in place for your safety, and the safety of fire aviation personnel, both in the air and on the ground.  He then proceeded to turn and walk away.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At 1751, MDC called and told me T-xx was en route from WYS to the incident, but that the fire had cancelled them. They wanted HLN aircraft to call T-xx and have him go directly to MSO instead of to the incident. AFF showed T-xx just SW of HLN. I called him on National Flight Following - no response at 1752. Tried again, 1753 - no response. 1753 - AIR GUARD contact attempted. No response. 1754, Tried contact on National Flight Following and again on AIR GUARD - no response. Icon went red on Automated Flight Following (AFF) screen. 1757, tried AIR GUARD again. No response. Called the HLN Tower. They had not seen T-xx in the skies (HLN tower does not have radar). A leadplane tried to raise him on NFF and on 125.125 (receiving incident''s Air-Air). I told Leadplane that the last point I had him on AFF was at 1739 (note time there - it is now 1758 on the clock), and relayed the last known position check: lat/long, heading 337 degrees @ 247 mph. Had MDC on the phone (to check the status of T-xx as far as they knew). They reported T-xx was ''yellow'' on their screen - relayed to leadplane. Moments later, MDC reported he''d gone ''red'' on her screen too. Relayed to Leadplane. Moments later, the lead successfully established contact with the tanker, who reported he was almost to the fire. HDC dispatcher checked with our Forest Aviation Officer, the GACC a/c desk (NRCC), neighboring dispatch center involved (MDC), as well as my center manager (HDC). All suggested a Safecom be filed for a number of related reasons, all centering on the fact that Air Guard is to be monitored at all times in aircraft, even when said a/c are employing Automated Flight Following. </t>
-  </si>
-  <si>
-    <t>May 16, 2001During flight operations over the Hurst Hammock fire the air attack pilot and the ATGS observed an intruder helicopter at their altitude (2000 ft MSL).  Sudden maneuvering was required to avoid collision.  The intruder aircraft then descended to 1500 ft and into the path of the lead plane.  The lead plane pilot then maneuvered to avoid collision and contacted ARTCC and asked if they were working a helicopter in the vicinity of the TFR over the fire.  ARTCC stated that they were not.  Lead maintained visual contact with the intruder aircraft and tanker operations were suspended until the intruder departed.  The aircraft maneuvered unpredictably in the vicinity of the fire, following the participating aircraft.  Positive identification was made that the intruder was a media helicopter and it was determined that he/she was maneuvering to photograph firefighting operations.  At one point the intruder departed the fire to film a fire-fighting helicopter dip water and then he/she chased the firefighting helo at the same altitude to the drop site.  All fire-fighting operations were ceased and the intruder departed.  Lead followed the intruder to class C airspace (approximately 2 mile to the East) and ensured that approach control had radar contact with the intruder aircraft.  Lead then coordinated with the fire and ATC to return to Pensacola Regional Airport to meet with the ARTCC supervisor.</t>
-  </si>
-  <si>
-    <t>After arriving to Cascade, ID from completing a mission on the bolder creek fire, the pilot and myself were advised that a potential hail storm was moving into the area. After refueling in Cascade to potentially fly to Boise, our alternate landing base, we received a mission from Cascade ID BOF to deliver food to the bolder creek fire. After discussing the incoming weather with the pilot, we decided we could complete the mission as it would take us out of the area, away from tracking storm, and allow us to circum navigate to Boise from the east/southeast. After the cargo mission was completed, we flight followed with Boise dispatch and asked for a weather update for the Ola helibase, our originally destination. They advised us of the same storm and suggested we not fly to Ola helibase. After discussing this with the pilot, we both concurred that the best course of action would be to continue to circumnavigate the storm to the east/southeast and continue to Boise. As we continued to circumnavigate the storm, we received an inflight weather briefing advising us of the storm tracking over the Ola helibase/Cascade area. During this time the weather was bumpy, there was no precipitation, and the visibility was 8-10 miles. About 40 miles out from Boise, we had a sudden on set of heavy rain. The exact words out of my mouth were “I hope that’s not hail,” and no later then finishing that sentence did we get hit by hail. The pilot immediately maneuvered the aircraft to the east and to a lower altitude, we continued to receive heavy rain for about another 15 -30 seconds before it ended. The whole incident lasted about a minute, from onset of rain to getting out of the hail. The flight continued to be bumpy but no other forms of precipitation was encountered for the rest of the flight. The first noticeable damage to the aircraft was the broken bubble window on the left door of the aircraft. After landing at Boise airport, the pilot, mechanic, and crew looked over the aircraft for damage. Damage to the aircraft consisted of the broken bubble window, divots in the skin on the nose, primarily isolated on the batter hatch cover, minor divots on the horizontal stabilizers leading edge, and divots on the upper vertical stabilizer. I notified my COR and Boise dispatch of what occurred. The pilot notified the company and further inspections by the OAS AMD’s will take place before becoming available for fire assignment.</t>
-  </si>
-  <si>
-    <t>On August 21st while returning from a recon of the Williams Butte fire on a Type 3 helicopter assigned to the fire, we spotted a jump ship flying up valley over the Foster Helibase. Immediately following, we saw a parachute in the trees below and another chute in the air at about 11 o’clock ahead. The pilot took immediate action turning to our right to avoid any additional conflict with the jumpers. Our flight path between Foster Helibase and the Williams Butte Fire was in constant use by as many as 11 helicopters on that date. The Williams Butte Fire had 4 type 1’s, 4 type 2’s, and 3 type 3’s. No communications were made by Wenatchee Dispatch (CWICC), the Smokejumper Base (NCSB), on a victor frequency by the jumpship to Foster helibase regarding the NCSB mission. Corrective Action: When a team is managing an incident on a Forest or other jurisdiction, close communication must be maintained between that jurisdiction’s aviation resources and the incident. Local jurisdiction on Initial Attack activities in the flight path of IMT aviation activities must be closely monitored. Frequencies need to be shared and commo exercised to ensure all aircraft are aware of others in the area. Somkejumpers should be assured that no other aircraft are in the same airspace</t>
-  </si>
-  <si>
-    <t>While enroute to the Duke Fire and West of Midland Texas the pilot tried to adjust the pitch on the {{{{{#}}}}}2 engine prop. The prop control failed at 2200 rpm. The pilot made the decision to return to Midland International Airfield to have the prop control checked. He then contacted the company mechanic who was enroute to meet the A/C in Midland. The mechanic found a broken wire at a solder point.</t>
-  </si>
-  <si>
-    <t>On July 20th at approximately 0916 air attack departed Redmond Tanker base to respond to Incident #0521 with pilot, air attack trainee and air attack instructor on board. Immediately after take-off, pilot in command informed air attack that we have a mechanical problem and we are returning to Redmond. After landing pilot informed air attack that the fuel flow gauge was inoperable and that he will take the plane to the local A&amp;P mechanic to inspect faulty gauge.</t>
+    <t>During departure with 2 nets weighing 1600lbs, NXXX did not gain enough altitude to clear the canopy north of the Helibase. Load calc at 7000 @ 25 was 1825lbs. Manager told pilot to return to cargo and place loads on deck, pilot did so. NXXXX than took different loads weighing less with no problem. Upon completion of mission the pilot realized he turned the pitch control setting (dial) 30 degrees in the wrong direction. He set it at -30 instead of +30. This caused the ship to show itself redlining while it still had enough power for the load.</t>
   </si>
   <si>
     <t>N1048Y was doing fire suppression bucket work on the Togo fire.  Ship was dipping water out of a 15,000 gallon heli-well with a Griffith bucket, at an established dip site about 2 miles south-east of the fire.  Ship had dipped out of the heli-well, and was beginning to depart the dip site when winds changed unfavorably. Consequently, ship had insufficent power/lift, so pilot dumped part of the water cargo.  The bucket came near (6-8 feet) to hitting ground as pilot was trying to regain lift, but the bucket did not hit ground.  The bucket was still part full (1/3 to 1/2) when pilot regained sufficient lift.  With a partially loaded bucket, pilot maneuvered ship back to the heli-well to again fill to capacity.  As pilot was positioning bucket over the heli-well to top it off to capacity, the partially loaded bucket came down on the rim of the heli-well.  The weight of the rigid bucket and water cargo buckled two panels of the heli-well, bending the panels inward, causing a slight overhang in the dip tank diameter.  Resulting damage may require replacing these two panels, if they cannot be bent back into shape.Note that damage only occurred to the heli-well, with no damage to N1048Y ship.</t>
   </si>
   <si>
-    <t>We, the smokejumper aircraft took runway 24 for takeoff and made our departure call on UNICOM.  Helitack helicopter said on UNICOM they were lifting from the ramp and would hold for our takeoff.  We started our takeoff roll and the helicopter departed to the north crossing runway 24 approximately 4,000 feet in front of us.  We called on UNICOM that we were already on our takeoff roll and the helicopter stated that they had us in sight.</t>
-  </si>
-  <si>
-    <t>notam</t>
-  </si>
-  <si>
-    <t>temporary flight restriction</t>
-  </si>
-  <si>
-    <t>confusion</t>
-  </si>
-  <si>
-    <t>collision</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> maneuver</t>
-  </si>
-  <si>
-    <t>airfield</t>
-  </si>
-  <si>
-    <t>trainee</t>
-  </si>
-  <si>
-    <t>[3, 7, 13, 39]</t>
-  </si>
-  <si>
-    <t>[7, 37]</t>
-  </si>
-  <si>
-    <t>[7, 14, 29, 39, 97]</t>
-  </si>
-  <si>
-    <t>[7, 14, 15, 24, 97]</t>
-  </si>
-  <si>
-    <t>[38, 65]</t>
-  </si>
-  <si>
-    <t>[27, 39, 58, 69, 80]</t>
-  </si>
-  <si>
-    <t>[36, 80, 88, 92]</t>
-  </si>
-  <si>
-    <t>[31, 34, 69, 72]</t>
-  </si>
-  <si>
-    <t>[8, 22, 51, 92]</t>
-  </si>
-  <si>
-    <t>[8, 11]</t>
+    <t>overload</t>
+  </si>
+  <si>
+    <t>load calc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> weight </t>
+  </si>
+  <si>
+    <t>[3, 63, 82]</t>
   </si>
   <si>
     <t>[3, 7, 63, 80, 88]</t>
   </si>
   <si>
-    <t>[7, 8, 82]</t>
-  </si>
-  <si>
-    <t>[39, 7]</t>
-  </si>
-  <si>
-    <t>[37, 7]</t>
-  </si>
-  <si>
-    <t>[65]</t>
-  </si>
-  <si>
-    <t>[27, 39, 69, 80]</t>
-  </si>
-  <si>
-    <t>[69, 31]</t>
-  </si>
-  <si>
-    <t>[7, 80]</t>
-  </si>
-  <si>
-    <t>97-0124</t>
-  </si>
-  <si>
-    <t>I was air attack Group Supervisor (AA6) flying over fire B441 talking to jump 17. We assigned them an altitude to come over the fire for a streamer pass while the air tanker was reloading. Jump17 finished his streamer run and started to climb without talking to us. We had jump 17 in sight at all times. Jay requested the pilot to notify air attack prior to changing elevations.</t>
-  </si>
-  <si>
-    <t>smokejumper</t>
-  </si>
-  <si>
-    <t>streamer</t>
-  </si>
-  <si>
-    <t>[34]</t>
-  </si>
-  <si>
-    <t>20-0733</t>
-  </si>
-  <si>
-    <t>01-0465</t>
-  </si>
-  <si>
-    <t>Approaching SBD for a load and return to the XXXXX Fire, TXXX had a bird strike on the underside of the right wing with damage to the outer flap tab hinge fairing. There was no damage to the actual mechanism.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">While flying recon on the Plumas NF I was about to call dispatch with adirection change when I noticed that radio #3 had gone off. I then triedto talk to the pilot and was unable to. I got his attention and then wenoticed that radio #2 had gone off. We then noticed the victor radio wasoff. We then started checking and found that the amp guage was showing adischarge. I called dispatch on my hand held radio and informed them thatwe lost the aircraft alternator and were in route to Quincy (Gansner)airport. The pilot turned off all other unnecessary electrical equipmentto save as much battery life as possibe. We were able to make a safe landing at Quincy airport even though we did not have any flaps. </t>
-  </si>
-  <si>
-    <t>flap</t>
-  </si>
-  <si>
-    <t>[2, 21, 23, 25]</t>
-  </si>
-  <si>
-    <t>[11, 14, 46, 74, 90]</t>
-  </si>
-  <si>
-    <t>[23]</t>
-  </si>
-  <si>
-    <t>04-0341</t>
-  </si>
-  <si>
-    <t>18-0517</t>
-  </si>
-  <si>
-    <t>05-0559</t>
-  </si>
-  <si>
-    <t>06-0519</t>
-  </si>
-  <si>
-    <t>15-0631</t>
-  </si>
-  <si>
-    <t>09-0269</t>
-  </si>
-  <si>
-    <t>01-0299</t>
-  </si>
-  <si>
-    <t>02-0566</t>
-  </si>
-  <si>
-    <t>16-0289</t>
-  </si>
-  <si>
-    <t>03-0497</t>
-  </si>
-  <si>
-    <t>16-0706</t>
-  </si>
-  <si>
-    <t>06-0331</t>
-  </si>
-  <si>
-    <t>08-0326</t>
-  </si>
-  <si>
-    <t>03-0781</t>
-  </si>
-  <si>
-    <t>00-0163</t>
-  </si>
-  <si>
-    <t>07-0833</t>
-  </si>
-  <si>
-    <t>11-0806</t>
-  </si>
-  <si>
-    <t>08-0578</t>
-  </si>
-  <si>
-    <t>11-0174</t>
-  </si>
-  <si>
-    <t>04-0434</t>
-  </si>
-  <si>
-    <t>02-0758</t>
-  </si>
-  <si>
-    <t>07-0608</t>
-  </si>
-  <si>
-    <t>16-0815</t>
-  </si>
-  <si>
-    <t>00-0698</t>
-  </si>
-  <si>
-    <t>13-0416</t>
-  </si>
-  <si>
-    <t>03-0192</t>
-  </si>
-  <si>
-    <t>03-1106</t>
-  </si>
-  <si>
-    <t>19-0126</t>
-  </si>
-  <si>
-    <t>After take-off, acft could not retract left main gear. Flight manual procedures were followed which directed the crew to lower the gear. A safe gear down and locked indication was displayed. Once a safe indication is indicated no further trouble shooting is allowed in flight. Flight engineer visually checked for safe indications thru inspection windows. Retardant was dumped at the fire site due to its proximity. Acft landed at IWA without incident.</t>
-  </si>
-  <si>
-    <t>WADNR UH-1H xxxxx was dispatched to the Ryegrass Coulee fire in the vicinity of Vantage, WA at 0730, 07/10/2018. xxxxx flew one fuel cycle and then landed at the helibase/ fuel site for a fuel and hold. At approximately 11:00 Air Attack requested xxxxx for bucket work, while lifting to leave the helibase a chip detector and warning light activated. The pilot contacted air attack and informed him the aircraft would be down for maintenance. xxxxx set down at the helibase, contacted agency mechanics and went through the proper procedures to isolate and remedy the issue. After the appropriate steps were taken the agency mechanic cleared xxxxx for incident operations. The aircraft finished up the day and returned to ellensburg base with no further issues.</t>
-  </si>
-  <si>
-    <t>NXXXX was flying air attack on the Burnt River Complex, over incident 154, call dispatch with a report that they lost an engine and were going to try to fly back to Baker on a single engine. At the time of engine failure, they were 22 miles out of Baker. Maintained Contact with NXXXX throughout the flight to Baker. They were able maintain altitude and land safely @ Baker without incident.Contacted Forest Aviation Officer and vendor. Also requested emergency response at the Baker Airport.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pilot failed to untie main rotor blades before start up. Pilot noticed that he did not untie at the same time he attempted to start engine. Immediately aborted start. Total time was approximately one second. Pilot untied blades and started helicopter. </t>
-  </si>
-  <si>
-    <t>Turbocharged 337 Cessna Skymaster pilot started the front engine without any problems. Attempted to start the rear engine but it would not start. The pilot followed other starting procedures as recommended by the owner but without success. The company mechanic was contacted and it was determined the fuel pump had failed. At 1900 aircraft was unavailable.</t>
-  </si>
-  <si>
-    <t>The helicopter departed CKX and upon arrival at the fire several warning lights{particle separator, rpm, engine 1 out, and engine 2 out} became illuminated. The pilot immediately began maneuvering toward the nearest landing spot, but all other gauges read normally &amp; we could still hear the engines running, so we returned to CKX. Enroute all warning lights except one paticle separator light went out. The helicopter landed without incident and the mechanic, IC, and AMD maintenance inspector were notified of the problem.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tanker 14 was responding to the Silent fire (RRU-47545) and developed an oil leak at the number three engine.  Tanker 14 then returned to SBD Tanker Base.  After inspection it was noted that an oil line was loose.  Oil line tightened, and aircraft put into contract availability.Gerry Burney notified and approved. </t>
-  </si>
-  <si>
-    <t>Dispatched as initial attack to a fire. Started acft engine and all appeared normal until the gas produced tachometer (N) went through 40%,I released the started switch and the engine flamed out, all indicationsof the start up to that point were normal.I contacted the DNR mechanic supervisor and he thought that perhaps thethrottle was rolled back a little to far off the detent to continuestarting sequence. Also, he said that there was the possibility of something similar to a vapor lock (air bubble) may have occured.I attempted a restart at his request and everything performednormally.After the restart Helicopter Manager contacted DNR Mechanic Supervisor once again to obtain clearance to resume operations. Clearancewas granted by mechanic.Helibase Manager contacted USFS to discuss start difficulties. After a conference between FS and DNR representatives Rotor 338 was fullyoperational.</t>
-  </si>
-  <si>
-    <t>We left the Airtanker Base at 1046 to do a requested Recon mission over the Galeuros and the Chirichua Ranges. We finished the Galeuros and were at the Dos Cabezas Mountains enroute to the Chrichuas when the pilot alerted me that the right engine tachometer needle was falling. I looked at the gauges and was a slow descent to 0 rpms. The pilot checked all the other gauges and they were all in the green. I visually looked at the right engine which showed no outward abnormalities. The pilot said that the xxx airport was close and we agreed that we would head the aircraft to there. Once that decision was made I called Dispatch and informed them that we had a malfunction with one of the gauges but operations were good and we were proceeding to the airport. We landed and went to maintenance facilities. Once parked, I notified Dispatch we were safe on the ground, and then notified management, and the OAS Maintenance Inspector of the situation.</t>
-  </si>
-  <si>
-    <t>Assign to lighting recon flight at 1050 Hrs. At end of planned flight, pilot noted right engine HP would not come back below 250 HP. Made landing at SBA at 1200 hrs. Mechanic worked on aircraft with test flight being OK. SZ Aviation Maintenace Inspector was called and aircraft was return to availability status. At 1549 hrs response to SB co fire #5209. 1615 hrs right engine would not come back below 250 HP, landed at SBA at 1641 hrs. SZ Maintenance Inspector was called on the situation, log book entry will be fax to Jerry when aircraft is returned to availability status.</t>
-  </si>
-  <si>
-    <t>Bird strike on engine number 1 noticed by crew chief on walk-around and discontinued reload for fire. Operations shut down. Pilots did not notice any engine concerns. Do not know the altitude, coordinates of strike or time it happened.</t>
-  </si>
-  <si>
-    <t>Aborted start on fire dispatch. Pilot attempted to start the aircraft with the battery cart. Initial voltage OK, upon spooling engine pilot noted excessive voltage drop. Not enough battery voltage to continue start. Pilot verified condition - low NG speed. Pilot followed proper procedure and correctly aborted start without any damage to aircraft.</t>
-  </si>
-  <si>
-    <t>On 6.16.2008 at approximately 1730 airtanker Lockheed P2 Neptune tail number xx was in the blocks and was under supervision of fixed wing parking tender. Aircraft had just completed loading retardent, loading crew was cleared, and airtanker was given permission to start engines. Pilot signaled to FWPT to clear him to start engine {#}2, clearance was given. As engine {#}2 was starting the suction from the propeller sucked a collapsible fabric and wire sunscreen out of the copilots window. The sunscreen disappeared with the engine blowby smoke behind the aircraft. Clearance was asked and given to start engine {#}1. As engine {#}1 cleared of smoke the sunscreen reappeared and swirled with the engine turbulence, threatening to be sucked into engine air intakes of both engine {#}1 and engine {#}2. Parking tender gave the pilot an emergency immediate cut-engine signal. Pilot responded immediately. The sunscreen fell to the ground in front of engine {#}2 and was retrieved by FWPT.</t>
-  </si>
-  <si>
-    <t>Pilot reported low fuel pressure indicator illuminated on the number 4 engine while over fire preparing for a drop.  PIC elected not to drop and returned to MFR for repairs.   Aircraft landed without incident.</t>
-  </si>
-  <si>
-    <t>After landing at KGCN for fuel the cowl of the right engine was observed to have a coating of grease that appeared to have come from the area of the propeller hub.  The aircraft had returned from spending 3.5 hours conducting leadplane activities on the Outlet Fire.</t>
-  </si>
-  <si>
-    <t>On takeoff fuel pressure gauges read normal, 10 minutes into the flight the right engine fuel pressure gauge was reading high. So the pilot decided to terminate the flight on return to the airport. aircraft was placed into contract unavailable status. Company maintenance chief decided to replace the right engine driven fuel pump and do the scheduled 50 hr inspection at the same time. During the inspection the mechanic found the right engine driven hydraulic pump had failed. Hydraulic pump was replaced 8/8/07.</t>
-  </si>
-  <si>
-    <t>Aircraft had an ‘Engine’ chip light starting up at Spring Creek Helibase and immediately shut back down.</t>
-  </si>
-  <si>
-    <t>Pilots heard a noise in the aft rotor system and a vibration upon returning to helibase, the aircraft was shut down while it was inspected by the mechanics, after inspection the mechanics advised the manager that the aircraft was out of service. There was a scheduled maintance to change the aft transmission the next day. The aircraft was made unavailable for the remainder of the afternoon.</t>
-  </si>
-  <si>
-    <t>After flying 4.6 hours on the Rockhouse Fire a transmission oil pressure warning light illuminated but transmission pressure indications were normal. Warning light is turned on by two pressure switches, one plumbed to the forward transmission and one on the aft transmission. This occured upon startup after refueling.</t>
-  </si>
-  <si>
-    <t>While performing large fire support on the Incident, an oil leak was discovered. Oil was dripping out of the valve and pooling in the carriage. 7/2/04 This narrative is an ammendment to the SAFECOM filed for this helicopter on 6/30/2004 (submitted by Helicopter Manager). Narrative: While performing a longline hookup I noticed a couple of puffs of white smoke come out of the left side cowl. I immediately had the pilot land and shut down the A/C. Upon inspection a leak was discovered on the breather tube flange that returns excess oil to the exhaust to be burned off. After discussion with the pilot it was determined that the helicopter needed to be repaired and that it would become un-available. I discussed the problem with my HELB(t) and we decided one of us needed to return to helibase to begin working on getting the helicopter repaired. The HELB(t) flew to helibase with the A/C. While I had confidence in the judgement of the pilot that the leak did not jeopardize the safety of the flight, I should have not asked the HELB(t) to fly down with the ship. This was a MAJOR oversight on my part. Policy dictates that when a problem is discovered that the A/C becomes unavailable @ that point. Once unavailable NO government personnel should be transported until the A/C is returned to service by an appropriate maintenance inspector.</t>
-  </si>
-  <si>
-    <t>Pilot reported low torque, inspection revealed fuel stream from P1 port in the inlet.  P1 bellows cracked.  Removed fuel control, installed fuel control with Allied Signal 1330.2 manual, chapter 73.  Put back into contract availability by the Regional Aviation Maintenance Inspector.</t>
-  </si>
-  <si>
-    <t>Pilot stated that he had an Engine/Airframe/Oil Filter Chip Light while on a Initial Attack mission. Pilot landed the aircraft and checked the chip plug and found very light fuzz on the plug. Pilot is an A/P mechanic.</t>
-  </si>
-  <si>
-    <t>Pilot attempted start of aircraft with main rotor tie down still in place. It was recognized prior to light off of engine by crew followed by immediate shut-down of starter generator.</t>
-  </si>
-  <si>
-    <t>The helicopter was getting ready to start and depart for the project site.  The pilot tried to start the helicopter and it did not.  He tried a second time and was uncessful.  He motioned to the fuel truck driver to bring out the APU and hook it up.  The pilot then tried a thrid time and determined the ignitor had gone bad.  Pilot called the office and had a mechanic dispatched.  A maintenance inspector was contacted and he said that in order to put the helicopter back in service the ignitor would have to be replaced and make a entry in the log book.</t>
-  </si>
-  <si>
-    <t>On duty at 0900, this would be day 3 for mission over site for the Fire within the Zone. At 0920 we did a aircraft systems check before departure and all ops normal, at 0941 we departed airport for the incident with: two souls, 4 1/2 hours of fuel, on a heading 214 degree`s for a 22 min, ETE to the incident. at this point all operations were normal and during this time was calculating the times for relief air attack over the fire. At 12 miles from incident contacted IA helicopter on victor for entry into the airspace of the fire TFR in place, we proceeded into the area at 10,000 dropping to 9,000 ft all ops normal. Established ground contact with operations and IC for operational update and reconfiguration of divisions from the previous day. ordered up fixed wing aircraft: 2 seats for retardant line across the west flank of the fire towards the head. All ops normal. about 3 3/4 hours into the flight the pilot noticed that the fuel use gauge that reads pounds of fuel used per sec was not operational for the right engine, the engine never quit running. The pilot re-calculated the weights and measures for passenger, fuel and cargo, determined that it was either a gauge failure or sending unit and we had plenty of fuel. At 1348 air attack relief was over the fire, did a brief on the tactics and division break downs and handed off to the relief air attack. We proceeded back to The designated base, all ops normal except for the faulty reading of the right fuel/use gauge. Landed safely, notified UAM and Dispatch that aircraft was unavailable due to gauge failure.</t>
-  </si>
-  <si>
-    <t>On the 2nd load of the morning, with the 2nd stick of rappellers, the engine fuel pump caution light came on.  The indicator light came on while the rappellers were on the skids, ready to exit the aircraft.  The pilot notified the spotter after the rappellers were on the ground and off the ropes, due to the fact that there was no fluctuation in fuel pressure.  The spotter disconnected ropes, closed doors and returned to the helipad.  Helicopter was then shutdown for inspection.</t>
-  </si>
-  <si>
-    <t>After refueling in Ely Nevada, XXX was enroute back to Battle Mountain Nevada.  Two minutes outside of Battle Mountain the pilot and I noticed the aroma of fuel.  Upon landing in Battle Mountain, we were in the process of parking the aircraft and noticed a fuel leak on the right side engine.  The pilot shut down the aircraft and made his inspections.  The problem appeared to be a broken fuel line.  The pilot then made calls to his company and mechanics.  I notified Battle Mountain Dispatch, WGBCC and Boise Smokejumpers Duty Officer.  Returned to service 7/1/03.  All repairs done at 0800.</t>
-  </si>
-  <si>
-    <t>As we were coming in to the LZ, one of the crew members on the ground noticed something leaking by the fuel tank. Once we landed and shut the helicopter down the pilot came and examined the leak. He said it was for sure fuel and we needed to find out where it was coming from. The pilot looked into the engine a little more and found out it was leaking between the electric fuel shut off valve. The pilot pressurized the system with the boost pumps and could not recreate the leak. He returned to base without the helitack crew.</t>
-  </si>
-  <si>
-    <t>engine</t>
-  </si>
-  <si>
-    <t>transmission</t>
-  </si>
-  <si>
-    <t>white smoke come</t>
-  </si>
-  <si>
-    <t>generator</t>
-  </si>
-  <si>
-    <t>[21, 30, 69, 83]</t>
-  </si>
-  <si>
-    <t>[33, 41, 50]</t>
-  </si>
-  <si>
-    <t>[7, 11, 59, 65, 69]</t>
-  </si>
-  <si>
-    <t>[29, 83]</t>
-  </si>
-  <si>
-    <t>[7, 88]</t>
-  </si>
-  <si>
-    <t>[73, 82, 85]</t>
-  </si>
-  <si>
-    <t>[8, 14, 67, 71, 97]</t>
-  </si>
-  <si>
-    <t>[55, 80, 83, 97]</t>
-  </si>
-  <si>
-    <t>[21, 43, 82]</t>
-  </si>
-  <si>
-    <t>[3, 69, 80]</t>
-  </si>
-  <si>
-    <t>[25, 41]</t>
-  </si>
-  <si>
-    <t>[13, 83]</t>
-  </si>
-  <si>
-    <t>[2, 8, 50, 88]</t>
-  </si>
-  <si>
-    <t>[8, 11, 41]</t>
-  </si>
-  <si>
-    <t>[3, 14, 23, 69, 97]</t>
-  </si>
-  <si>
-    <t>[53, 67, 82]</t>
-  </si>
-  <si>
-    <t>[80, 93]</t>
-  </si>
-  <si>
-    <t>[24, 74]</t>
-  </si>
-  <si>
-    <t>[50, 53, 58, 85]</t>
-  </si>
-  <si>
-    <t>[64, 67, 68, 80]</t>
-  </si>
-  <si>
-    <t>[7, 23, 43, 97]</t>
-  </si>
-  <si>
-    <t>[50, 80]</t>
-  </si>
-  <si>
-    <t>[11, 22, 58, 68, 97]</t>
-  </si>
-  <si>
-    <t>[63, 83]</t>
-  </si>
-  <si>
-    <t>[3, 41, 53, 97]</t>
-  </si>
-  <si>
-    <t>[8, 53, 67]</t>
-  </si>
-  <si>
-    <t>[41, 67, 88]</t>
-  </si>
-  <si>
-    <t>[50, 41]</t>
-  </si>
-  <si>
-    <t>[8, 97]</t>
-  </si>
-  <si>
-    <t>[83, 97]</t>
-  </si>
-  <si>
-    <t>[41]</t>
-  </si>
-  <si>
-    <t>[50, 8]</t>
-  </si>
-  <si>
-    <t>[8, 41]</t>
-  </si>
-  <si>
-    <t>[97]</t>
-  </si>
-  <si>
-    <t>[50]</t>
-  </si>
-  <si>
-    <t>[64]</t>
-  </si>
-  <si>
-    <t>[41, 97]</t>
-  </si>
-  <si>
-    <t>00-0509</t>
-  </si>
-  <si>
-    <t>Subject:  SAFECOM - Canadian Bird Dog#52,           Left Engine Failure.At approximately 1100 hours MDT Canadian Bird Dog#52, a Turbo Commander, departed Miles City, Montana for Helena, MT.  After reaching cruising altitude of 12,500 feet westbound, and 25 minutes out of Miles City, the left engine suddenly lost power and went to auto feather.  There were no prior indications (instrumentation) that there was a problem developing.  After a cool down period of approximately 2 minutes, and attempt to restart the engine was made but immediately aborted due to no indication of oil pressure.The aircraft was under FS flight following with Lewistown as Billings could not be raised.  Flight following and position reports were also conveyed to Helena on FS nets.The aircraft had no difficulty maintaining altitude and was operating in CAVU conditions.  The flight crew made a judgement call to continue on to Missoula where they had maintenance support even though it was somewhat further than Helena where the logistics of repair would be difficult.  This decision was based on what the flight crew believed to be inpracticablein given the circumstances of clear air, no problems in maintaining altitude, other available landing places along the route, and the availability of maintenance support in Missoula.Bird Dog #52 continued west at 12,500 feet MSL with no further difficulties, other than reduced airspeed, and maintained visuals on airports and landing area's they could reach if problems developed with the right engine.Landing was affected in Missoula at near 1200 hours where they taxied to Northstar Aviation and met with their maintenance team.  The cowling was removed, screens pulled showing a lot of evidence of metal particle, i.e., steel and brass.  The engine had failed and required an engine change.USDA Forest Service LiaisonCanadian Airtanker Deployment</t>
-  </si>
-  <si>
-    <t>oil</t>
-  </si>
-  <si>
-    <t>[8, 14, 62, 80, 82]</t>
-  </si>
-  <si>
-    <t>07-0629</t>
-  </si>
-  <si>
-    <t>During departure with 2 nets weighing 1600lbs, NXXX did not gain enough altitude to clear the canopy north of the Helibase. Load calc at 7000 @ 25 was 1825lbs. Manager told pilot to return to cargo and place loads on deck, pilot did so. NXXXX than took different loads weighing less with no problem. Upon completion of mission the pilot realized he turned the pitch control setting (dial) 30 degrees in the wrong direction. He set it at -30 instead of +30. This caused the ship to show itself redlining while it still had enough power for the load.</t>
-  </si>
-  <si>
-    <t>load calc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> weight </t>
-  </si>
-  <si>
-    <t>[3, 63, 82]</t>
-  </si>
-  <si>
     <t>[63]</t>
   </si>
   <si>
@@ -1558,15 +1567,30 @@
     <t>[56]</t>
   </si>
   <si>
+    <t>05-0739</t>
+  </si>
+  <si>
     <t>00-0573</t>
   </si>
   <si>
+    <t xml:space="preserve">Our helicopter and crew was dispatched to IA a fire on the north end of the District. Upon arrival we discovered 2 civilians near the heel of the fire, along with a vehicle inside the fire perimeter that had been consumed by fire. After landing near the two individuals, I asked them about the situation, I was informed that their vechicle had started the fire. I made the decision to fly them off the fire to the Carey airstrip without full PPE(except for flight helmets) because of several reasons:(1)they were in danger of being over-run by the fire,(2)they were experiencing health problems, probably due to dehydration and (3)they were in the middle of the desert without food, water, or transportation.  </t>
+  </si>
+  <si>
     <t xml:space="preserve">116 was enroute back from the fire to the helibase for water and noticed a 206-L3 flying 300-400' AGL just south of the helibase.  No evasive maneuvers were needed.  Helibase personnel recognized the L3 as a Globe medivac ship. </t>
   </si>
   <si>
+    <t>ems</t>
+  </si>
+  <si>
+    <t>[6, 68, 98]</t>
+  </si>
+  <si>
     <t>[7, 14, 69, 80, 97]</t>
   </si>
   <si>
+    <t>[98]</t>
+  </si>
+  <si>
     <t>13-0868</t>
   </si>
   <si>
@@ -1630,112 +1654,61 @@
     <t>[55, 55]</t>
   </si>
   <si>
-    <t>13-0415</t>
-  </si>
-  <si>
-    <t>14-0601</t>
-  </si>
-  <si>
-    <t>02-0619</t>
-  </si>
-  <si>
-    <t>13-0619</t>
-  </si>
-  <si>
-    <t>00-0689</t>
-  </si>
-  <si>
-    <t>13-0438</t>
-  </si>
-  <si>
-    <t>08-0212</t>
+    <t>03-0995</t>
+  </si>
+  <si>
+    <t>04-0654</t>
   </si>
   <si>
     <t>18-0633</t>
   </si>
   <si>
-    <t>02-1289</t>
-  </si>
-  <si>
     <t>08-0924</t>
   </si>
   <si>
-    <t>On July 1, at approximately 2000 while on approach for Designated base, the aircraft struck a bird. The impact occurred on the front center{nose}of the helicopter and the bird departed up and to the pilot side {left} of the windscreen. Damage to the nose cone includes 2 cracks thru the skin of the nose cone, each approximately 7 inches in length, one vertical on the left side of the impact area, and one horizontal crack across the bottom of the impact area, viewed from the perspective of one looking at the nose cone from the front of the aircraft. No other damage other than these cracks was noted. The bird species unknown, but did not seem to be particularly large for the split second it was observed before impact.</t>
-  </si>
-  <si>
-    <t>Aircraft had performed multiple crew shuttles as well as a cycle of bucket work on two fires that were in close proximity to each other. Aircraft set down for fuel at local IA helibase and was shut down preparing to shuttle additional FFTR’s into Fire. Helitack personnel opened right rear door to load gear and door dropped due to only being attached by the lower door pin. Upper door pin was missing. Helitack caught door preventing it from being damaged. How the pin became dislodged or when is unknown. Cause of the pin to become missing is also unknown, but previous inspections have revealed one of two ball bearings missing that could potentially allow for the pin to back its way out of the door hinge.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     HELICOPTER XXX, AN S-64 SKYCRANE WITH INTERNAL TANK ANDSNORKLE, WAS DOING WATER DROPS ON THE BOULDER FIRE ON 7/27/02.  UPONSHUTDOWN ON LAST SORTIE OF THE DAY, THE PILOT AND MAINTENANCE CREW CAMEOVER AND REPORTED A NEED TO REPLACE A DELAMINATING ROTOR BLADE.  THEREHAD BEEN NO STRIKE OR ACCIDENT REPORTED PRIOR.       AN INSPECTION OF THE BLADE REVEALED A 2inX4in PEEL BACK ON THE BOTTOMOF ONE ROTOR BLADE ABOUT ONE THIRD OF THE WAY DOWN FROM THE TIP. THE PEELTURNS OUTWARD AND LOOKS LIKE A inTEAR TO THE SHEETMETALin.  THE SPAR UNDERIT IS VISIBLE AND APPEARS UNDAMAGED.  THE BIMS READS WHITE, INDICATINGNO LOSS OF PRESSURE.  THE CREW REPORTED IT AS SOON AS IT WAS DISCOVERED,ABOUT 2030 HOURS.</t>
-  </si>
-  <si>
-    <t>During a routine preflight inspection in the morning 7/26, I noticed a divot in the left propeller. The divot was located on the leading edge, approximately 5 inches from the prop tip and was roughly the length of a penny in width and half a penny in depth. I grounded the aircraft until further notice and reported the discrepancy to my supervisor and the persons responsible for maintenance of the aircraft. I believe the damage was caused from a rock or bolt making contact with the prop during landing or taxi. A factor which likely contributed to the FOD damage was darkness, as I landed 20 minutes after sunset the previous night. Exacerbating the darkness factor are the lights in the Cedar City ATB light fixed wing parking area, which shine from the ground up, directly into the pilot````s eyes during taxi/parking operations. A parking tender was present, which helped. A factor which may have led to the FOD in the first place may have been the path used by vehicles between the main tanker base vehicle parking lot and the light fixed wing ramp. The path short cuts the paved route to the ramp via a loose gravel two track. See attached images for FOD damages and dirt path shortcut.</t>
-  </si>
-  <si>
-    <t>H534 was inbound to Mill Creek Helibase after a water dropping missison on the East Fire.  While landing the Pilot landed the helicoptors' snorkel toofar forward under neath the fixed tank.  The fixed tank has a 50 gallon fiberglass extension on it behind the standard 300 gallon steel tank.  The result was a horseshoe size crack on the fiberglass extension. A parking tender was in place at the time, but he was too for back and the skidswere above eye level.  Parking tender informed the manager of the incident.  The helicoptor manager informed the parking tender that he should of been a little bit closer, so he could see the position of the snorkel in regards to the fixed tank.  The tank was repared with no difficulty at all.  The Pilot also stated that he would pay more attention the the position of the snorkel while landing.</t>
-  </si>
-  <si>
-    <t>After a Ferry Flight lasting 30 minutes, and during post flight inspection performed by the mechanics, a blade delimitation {a bubble approximatly 8 inches long by 3 inches wide} was found at the underside and outer 1/4 of the right blade. The inspection revealed the delamination was due to what appeared to be a manufacture defect. The Pilot was consulted and reported no unusual or abnormal flight characteristics during the ferry flight. Mechanic informed the Helicopter Manager of the situation and made the aircraft unavailable.</t>
-  </si>
-  <si>
-    <t>While performing a routine maintenance inspection on the aircraft following a water dropping mission on the fire the mechanic discovered that the tail rotor box on the aircraft was cracked. The aircraft was made unavailable until a new tail rotor box could be installed.</t>
+    <t>06-1277</t>
+  </si>
+  <si>
+    <t>During preflight pilot found a crack in the exhaust cone         near the attachment clamp. The exhaust cone was removed          from service. Aircraft was unavailable.</t>
+  </si>
+  <si>
+    <t>After returning from the XXXXXXX Fire, the pilot fueled the aircraft and then proceeded to taxi across the runway to the Tanker Base. During the taxi, the right engine stalled. A restart was attempted and failed. Subsequent inspection revealed that 2-3 wires were burned and arced inside the engine compartment apparently from exposure to extreme heat from the turbocharger. On 7/28/2004 The wires were replaced and re-routed away from the turbocharger to prevent additional occurences. A test flight was attempted but the right engine mag test failed. Subsequent tests revealed that some spark plugs were fouled/replaced and the test flight was accomplished. Upon return from the flight the pilot opened the cowls for an inspection and discovered hot air coming from the side of the turbocharger waste gate (possibly the original cause of the burned wires). The FS Mechanic Inspector was notified and recommended a closer look at the exhaust components. It was found that the crack in the right engine turbo waste gate was adjcent to an old weld repair. Further inspection from the FS Mechanic revealed no heat shields installed and several repairs were evident on the existing exhaust parts.</t>
   </si>
   <si>
     <t>When T-XX was returning off the Bruneau fire PIC reported a bird strike. Upon landing in TWF, crew chief conducted an inspection. Bird remains were found on the 2nd right pylon. Crew Chief pulled the panel to ensure no damage. COR notified and COR Contacted AMI. No damage was found during inspection. Maintenance inspector returned aircraft returned to service @ 1530</t>
   </si>
   <si>
-    <t>Upon doing pre-use inspection I noticed fuel on the ground.  After looking closer, there was a leak on the fuel tank on the support/service trailer.  The leak was located on the lower right side of the tank.  A previous impact to the tank appeared to have created a crack that had rusted and a leak start.</t>
-  </si>
-  <si>
     <t>On assignment for the Lonesome Complex the aircraft was ordered up with a bucket. The Helicopter is equiped with a fixed tank under the exclusive-use National Helicopter contract and within section B-12 is necessary to have a variable capacity collapsible bucket as an addition or back-up with the fixed-tank helicopter. The contracted fixed-tank helicopter has along with it a FAST {Fire Attack Storm Tank} Bucket, manufactured by Absolute Fire Solutions, INC and distributed by Simplex MFG. While making a dip at the dip site, one of the purse string wires hooked underneath the bolts rubber stopper and nut on the metal frame; this resulting in the frame bending under the added stress to the frame itself rather than the anchor points as intended. The frame was bent in a twisting manor and the purse string wire had groves {ware} along it showing that it caught on ''something'' with an edge.</t>
   </si>
   <si>
-    <t xml:space="preserve"> damage</t>
-  </si>
-  <si>
-    <t>tear</t>
-  </si>
-  <si>
-    <t>crack</t>
-  </si>
-  <si>
-    <t>delamination</t>
+    <t>The pilot of 28M noticed that the main cabin door had play in the door hinge and some of the rivets had started to pull through the sheet metal.  It was brought to the attention of maintenance and the door was removed for inspection.  Maintenance found several rivets that had pulled through the sheet metal that covers the outside of the door and the metal door hinge had ripped several inches on the aft section of the hinge.</t>
+  </si>
+  <si>
+    <t>weld</t>
   </si>
   <si>
     <t>pylon</t>
   </si>
   <si>
-    <t>bent</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> wing</t>
-  </si>
-  <si>
-    <t>[23, 25]</t>
-  </si>
-  <si>
-    <t>[23, 72, 88]</t>
-  </si>
-  <si>
-    <t>[3, 23, 37, 62, 67]</t>
-  </si>
-  <si>
-    <t>[2, 12, 23]</t>
-  </si>
-  <si>
-    <t>[3, 23, 31, 70, 80]</t>
-  </si>
-  <si>
-    <t>[23, 80]</t>
+    <t>metal frame</t>
+  </si>
+  <si>
+    <t>sheet metal</t>
+  </si>
+  <si>
+    <t>[23, 69, 80]</t>
+  </si>
+  <si>
+    <t>[8, 22, 23, 54, 82]</t>
   </si>
   <si>
     <t>[23, 24]</t>
   </si>
   <si>
-    <t>[18, 23, 69, 97]</t>
-  </si>
-  <si>
     <t>[3, 23, 35, 68, 81]</t>
+  </si>
+  <si>
+    <t>[23, 88]</t>
   </si>
   <si>
     <t>[23, 35]</t>
@@ -2282,7 +2255,7 @@
         <v>174</v>
       </c>
       <c r="E2" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="F2" t="s">
         <v>198</v>
@@ -2293,7 +2266,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2302,21 +2275,21 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E3" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="F3" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="G3" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2325,13 +2298,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -2339,7 +2312,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2348,21 +2321,21 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="G5" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2371,21 +2344,21 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="E6" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="F6" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="G6" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2394,21 +2367,21 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E7" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="F7" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="G7" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2417,21 +2390,21 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="E8" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="F8" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="G8" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2440,21 +2413,21 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="G9" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2463,21 +2436,21 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="G10" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2486,10 +2459,10 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E11" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="F11" t="s">
         <v>143</v>
@@ -2541,7 +2514,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2572,7 +2545,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2581,21 +2554,21 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="E2" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="F2" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="G2" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2604,13 +2577,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -2618,7 +2591,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2627,13 +2600,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="G4" t="s">
         <v>71</v>
@@ -2653,7 +2626,7 @@
         <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="F5" t="s">
         <v>73</v>
@@ -2664,7 +2637,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2673,13 +2646,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="E6" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="F6" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="G6" t="s">
         <v>71</v>
@@ -2687,7 +2660,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>293</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2696,21 +2669,21 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>300</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="F7" t="s">
-        <v>310</v>
+        <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>313</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2719,21 +2692,21 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="E8" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="F8" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2742,16 +2715,39 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="E9" t="s">
+        <v>314</v>
+      </c>
+      <c r="F9" t="s">
+        <v>320</v>
+      </c>
+      <c r="G9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F9" t="s">
-        <v>312</v>
-      </c>
-      <c r="G9" t="s">
-        <v>314</v>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>310</v>
+      </c>
+      <c r="E10" t="s">
+        <v>311</v>
+      </c>
+      <c r="F10" t="s">
+        <v>321</v>
+      </c>
+      <c r="G10" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -2761,7 +2757,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2792,7 +2788,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2801,44 +2797,44 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="E2" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="F2" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="G2" t="s">
-        <v>358</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="E3" t="s">
-        <v>340</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="G3" t="s">
-        <v>359</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>326</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2847,13 +2843,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>337</v>
       </c>
       <c r="E4" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>354</v>
       </c>
       <c r="G4" t="s">
         <v>147</v>
@@ -2861,99 +2857,99 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>253</v>
+        <v>327</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>262</v>
+        <v>338</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>347</v>
       </c>
       <c r="F5" t="s">
-        <v>277</v>
+        <v>355</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>317</v>
+        <v>26</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>329</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>339</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>348</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="E7" t="s">
-        <v>339</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="F8" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="G8" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>320</v>
+        <v>85</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2962,44 +2958,44 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>332</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="F9" t="s">
-        <v>351</v>
+        <v>97</v>
       </c>
       <c r="G9" t="s">
-        <v>361</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>321</v>
+        <v>158</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>333</v>
+        <v>180</v>
       </c>
       <c r="E10" t="s">
-        <v>343</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>352</v>
+        <v>204</v>
       </c>
       <c r="G10" t="s">
-        <v>147</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3008,21 +3004,21 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="G11" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3031,13 +3027,13 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="E12" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="F12" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="G12" t="s">
         <v>101</v>
@@ -3045,7 +3041,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3054,13 +3050,13 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="E13" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="F13" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="G13" t="s">
         <v>101</v>
@@ -3068,7 +3064,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>325</v>
+        <v>246</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3077,44 +3073,44 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>337</v>
+        <v>250</v>
       </c>
       <c r="E14" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="F14" t="s">
-        <v>356</v>
+        <v>257</v>
       </c>
       <c r="G14" t="s">
-        <v>363</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>238</v>
+        <v>28</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>242</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>345</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>249</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3123,15 +3119,38 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="G16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>345</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>362</v>
+      </c>
+      <c r="G17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3178,7 +3197,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3232,7 +3251,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>322</v>
+        <v>368</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3241,39 +3260,16 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>334</v>
+        <v>369</v>
       </c>
       <c r="E3" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="F3" t="s">
-        <v>353</v>
+        <v>133</v>
       </c>
       <c r="G3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>365</v>
-      </c>
-      <c r="E4" t="s">
-        <v>367</v>
-      </c>
-      <c r="F4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G4" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -3314,7 +3310,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3323,21 +3319,21 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="E2" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="F2" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="G2" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3346,13 +3342,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="E3" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="F3" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="G3" t="s">
         <v>217</v>
@@ -3432,7 +3428,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>377</v>
+        <v>324</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3441,21 +3437,21 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>405</v>
+        <v>335</v>
       </c>
       <c r="E2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F2" t="s">
-        <v>437</v>
+        <v>352</v>
       </c>
       <c r="G2" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3464,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -3473,12 +3469,12 @@
         <v>438</v>
       </c>
       <c r="G3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3487,7 +3483,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -3501,7 +3497,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3510,21 +3506,21 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E5" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F5" t="s">
         <v>440</v>
       </c>
       <c r="G5" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3533,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -3547,7 +3543,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3556,10 +3552,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E7" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F7" t="s">
         <v>442</v>
@@ -3570,7 +3566,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3579,21 +3575,21 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E8" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F8" t="s">
         <v>443</v>
       </c>
       <c r="G8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3602,7 +3598,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -3611,12 +3607,12 @@
         <v>444</v>
       </c>
       <c r="G9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3625,10 +3621,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E10" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F10" t="s">
         <v>445</v>
@@ -3651,7 +3647,7 @@
         <v>176</v>
       </c>
       <c r="E11" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F11" t="s">
         <v>200</v>
@@ -3662,7 +3658,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3671,13 +3667,13 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>446</v>
+        <v>240</v>
       </c>
       <c r="G12" t="s">
         <v>23</v>
@@ -3685,7 +3681,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3694,21 +3690,21 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E13" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G13" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3717,21 +3713,21 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E14" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G14" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3740,21 +3736,21 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E15" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -3763,16 +3759,16 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E16" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G16" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3789,18 +3785,18 @@
         <v>182</v>
       </c>
       <c r="E17" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F17" t="s">
         <v>206</v>
       </c>
       <c r="G17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3809,21 +3805,21 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E18" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F18" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G18" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3832,13 +3828,13 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G19" t="s">
         <v>220</v>
@@ -3846,7 +3842,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3855,13 +3851,13 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G20" t="s">
         <v>219</v>
@@ -3869,7 +3865,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3878,13 +3874,13 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G21" t="s">
         <v>23</v>
@@ -3892,7 +3888,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3901,21 +3897,21 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E22" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F22" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G22" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -3924,21 +3920,21 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E23" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F23" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G23" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3947,21 +3943,21 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G24" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3970,21 +3966,21 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G25" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -3993,21 +3989,21 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="E26" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F26" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="G26" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4016,21 +4012,21 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E27" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F27" t="s">
         <v>440</v>
       </c>
       <c r="G27" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4039,21 +4035,21 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E28" t="s">
         <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G28" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4062,16 +4058,16 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E29" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F29" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G29" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -4088,7 +4084,7 @@
         <v>66</v>
       </c>
       <c r="E30" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F30" t="s">
         <v>78</v>
@@ -4099,7 +4095,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4108,21 +4104,21 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E31" t="s">
         <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G31" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -4131,13 +4127,13 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E32" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F32" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G32" t="s">
         <v>101</v>
@@ -4145,7 +4141,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -4154,16 +4150,16 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F33" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G33" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -4204,22 +4200,22 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>474</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>475</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>476</v>
-      </c>
-      <c r="F2" t="s">
-        <v>477</v>
       </c>
       <c r="G2" t="s">
         <v>220</v>
@@ -4429,7 +4425,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4460,7 +4456,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>478</v>
+        <v>85</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -4469,21 +4465,21 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>479</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F2" t="s">
-        <v>482</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>483</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>325</v>
+        <v>477</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4492,16 +4488,39 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>337</v>
+        <v>479</v>
       </c>
       <c r="E3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F3" t="s">
-        <v>356</v>
+        <v>484</v>
       </c>
       <c r="G3" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>480</v>
+      </c>
+      <c r="E4" t="s">
         <v>483</v>
+      </c>
+      <c r="F4" t="s">
+        <v>485</v>
+      </c>
+      <c r="G4" t="s">
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -4542,7 +4561,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -4551,21 +4570,21 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="E2" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="F2" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="G2" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4574,21 +4593,21 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="E3" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="F3" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="G3" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4597,21 +4616,21 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="E4" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="F4" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="G4" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4620,16 +4639,16 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="E5" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="F5" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="G5" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -4675,7 +4694,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4706,24 +4725,47 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="E2" t="s">
+        <v>508</v>
+      </c>
+      <c r="F2" t="s">
+        <v>509</v>
+      </c>
+      <c r="G2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>507</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>503</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F3" t="s">
+        <v>510</v>
+      </c>
+      <c r="G3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4765,7 +4807,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>504</v>
+        <v>512</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -4774,21 +4816,21 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>509</v>
+        <v>517</v>
       </c>
       <c r="E2" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="F2" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="G2" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4797,21 +4839,21 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="G3" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4820,21 +4862,21 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>518</v>
+        <v>526</v>
       </c>
       <c r="G4" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4843,7 +4885,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -4869,18 +4911,18 @@
         <v>177</v>
       </c>
       <c r="E6" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="F6" t="s">
         <v>201</v>
       </c>
       <c r="G6" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4889,21 +4931,21 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="E7" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="F7" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="G7" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4912,21 +4954,21 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G8" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4935,16 +4977,16 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="G9" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -4954,7 +4996,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4985,7 +5027,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4994,21 +5036,21 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="G2" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5017,21 +5059,21 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="E3" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F3" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="G3" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5040,21 +5082,21 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="E4" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F4" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="G4" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5063,21 +5105,21 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="E5" t="s">
         <v>545</v>
       </c>
       <c r="F5" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="G5" t="s">
-        <v>376</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5086,154 +5128,16 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="E6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F6" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="G6" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>540</v>
-      </c>
-      <c r="E7" t="s">
-        <v>548</v>
-      </c>
-      <c r="F7" t="s">
-        <v>376</v>
-      </c>
-      <c r="G7" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>541</v>
-      </c>
-      <c r="E8" t="s">
-        <v>547</v>
-      </c>
-      <c r="F8" t="s">
-        <v>557</v>
-      </c>
-      <c r="G8" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>542</v>
-      </c>
-      <c r="E9" t="s">
-        <v>549</v>
-      </c>
-      <c r="F9" t="s">
-        <v>558</v>
-      </c>
-      <c r="G9" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>543</v>
-      </c>
-      <c r="E10" t="s">
-        <v>547</v>
-      </c>
-      <c r="F10" t="s">
-        <v>559</v>
-      </c>
-      <c r="G10" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>544</v>
-      </c>
-      <c r="E11" t="s">
-        <v>550</v>
-      </c>
-      <c r="F11" t="s">
-        <v>560</v>
-      </c>
-      <c r="G11" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>242</v>
-      </c>
-      <c r="E12" t="s">
-        <v>551</v>
-      </c>
-      <c r="F12" t="s">
-        <v>249</v>
-      </c>
-      <c r="G12" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -5286,7 +5190,7 @@
         <v>176</v>
       </c>
       <c r="E2" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="F2" t="s">
         <v>200</v>
@@ -5297,7 +5201,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5306,16 +5210,16 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="E3" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
       <c r="F3" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="G3" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -6724,7 +6628,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6764,16 +6668,62 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>239</v>
+      </c>
+      <c r="G3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="F2" t="s">
-        <v>233</v>
-      </c>
-      <c r="G2" t="s">
-        <v>234</v>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G4" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -6814,7 +6764,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -6823,21 +6773,21 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="E2" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="F2" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="G2" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6846,21 +6796,21 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="E3" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="F3" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="G3" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -6869,13 +6819,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -6883,7 +6833,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -6892,13 +6842,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="E5" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="F5" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="G5" t="s">
         <v>217</v>

</xml_diff>